<commit_message>
change data frame to be able to show square, position, row, column in excel sheet
</commit_message>
<xml_diff>
--- a/empty_board.xlsx
+++ b/empty_board.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\03_research_and_development\03_emans_projects\02_my_ideas_and_projects\project_63_sudoku\sudoku_version_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B2349D62-B7DC-48A5-82BD-DD3FF243E577}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF35B68A-0896-4A57-BB59-063B005EE646}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{7640EADC-91D7-4D8B-898E-027899374FBD}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{7640EADC-91D7-4D8B-898E-027899374FBD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="45">
   <si>
     <t xml:space="preserve"> ___ ___ ___ ___ </t>
   </si>
@@ -123,6 +123,54 @@
   </si>
   <si>
     <t>spacer_8</t>
+  </si>
+  <si>
+    <t>TR - P1 - R1 - C1</t>
+  </si>
+  <si>
+    <t>TR - P3 - R2 - C1</t>
+  </si>
+  <si>
+    <t>BR - P1 - R3 - C1</t>
+  </si>
+  <si>
+    <t>BR - P3 - R4 - C1</t>
+  </si>
+  <si>
+    <t>BR - P4 - R4 - C2</t>
+  </si>
+  <si>
+    <t>BR - P2 - R3 - C2</t>
+  </si>
+  <si>
+    <t>TR - P4 - R2 - C2</t>
+  </si>
+  <si>
+    <t>TR - P2 - R1 - C2</t>
+  </si>
+  <si>
+    <t>TL - P2 - R1 - C4</t>
+  </si>
+  <si>
+    <t>TL - P4 - R2 - C4</t>
+  </si>
+  <si>
+    <t>BL - P2 - R3 - C4</t>
+  </si>
+  <si>
+    <t>BL - P4 - R4 - C4</t>
+  </si>
+  <si>
+    <t>TL - P1 - R1 - C3</t>
+  </si>
+  <si>
+    <t>BL - P1 - R3 - C3</t>
+  </si>
+  <si>
+    <t>BL - P3 - R4 - C3</t>
+  </si>
+  <si>
+    <t>TL - P3 - R2 - C3</t>
   </si>
 </sst>
 </file>
@@ -486,32 +534,32 @@
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="37.140625" customWidth="1"/>
+    <col min="1" max="1" width="37.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -526,12 +574,18 @@
   <dimension ref="A1:R6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+      <selection activeCell="P1" sqref="P1:P1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="4" max="4" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.90625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.6328125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.6328125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -587,7 +641,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
         <v>4</v>
       </c>
@@ -640,7 +694,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -650,8 +704,8 @@
       <c r="C3" t="s">
         <v>5</v>
       </c>
-      <c r="D3">
-        <v>1</v>
+      <c r="D3" t="s">
+        <v>29</v>
       </c>
       <c r="E3" t="s">
         <v>5</v>
@@ -662,8 +716,8 @@
       <c r="G3" t="s">
         <v>5</v>
       </c>
-      <c r="H3">
-        <v>2</v>
+      <c r="H3" t="s">
+        <v>36</v>
       </c>
       <c r="I3" t="s">
         <v>5</v>
@@ -674,8 +728,8 @@
       <c r="K3" t="s">
         <v>5</v>
       </c>
-      <c r="L3">
-        <v>1</v>
+      <c r="L3" t="s">
+        <v>41</v>
       </c>
       <c r="M3" t="s">
         <v>5</v>
@@ -686,8 +740,8 @@
       <c r="O3" t="s">
         <v>5</v>
       </c>
-      <c r="P3">
-        <v>2</v>
+      <c r="P3" t="s">
+        <v>37</v>
       </c>
       <c r="Q3" t="s">
         <v>5</v>
@@ -696,7 +750,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -706,8 +760,8 @@
       <c r="C4" t="s">
         <v>5</v>
       </c>
-      <c r="D4">
-        <v>3</v>
+      <c r="D4" t="s">
+        <v>30</v>
       </c>
       <c r="E4" t="s">
         <v>5</v>
@@ -718,8 +772,8 @@
       <c r="G4" t="s">
         <v>5</v>
       </c>
-      <c r="H4">
-        <v>4</v>
+      <c r="H4" t="s">
+        <v>35</v>
       </c>
       <c r="I4" t="s">
         <v>5</v>
@@ -730,8 +784,8 @@
       <c r="K4" t="s">
         <v>5</v>
       </c>
-      <c r="L4">
-        <v>3</v>
+      <c r="L4" t="s">
+        <v>44</v>
       </c>
       <c r="M4" t="s">
         <v>5</v>
@@ -742,8 +796,8 @@
       <c r="O4" t="s">
         <v>5</v>
       </c>
-      <c r="P4">
-        <v>4</v>
+      <c r="P4" t="s">
+        <v>38</v>
       </c>
       <c r="Q4" t="s">
         <v>5</v>
@@ -752,7 +806,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -762,8 +816,8 @@
       <c r="C5" t="s">
         <v>5</v>
       </c>
-      <c r="D5">
-        <v>1</v>
+      <c r="D5" t="s">
+        <v>31</v>
       </c>
       <c r="E5" t="s">
         <v>5</v>
@@ -774,8 +828,8 @@
       <c r="G5" t="s">
         <v>5</v>
       </c>
-      <c r="H5">
-        <v>2</v>
+      <c r="H5" t="s">
+        <v>34</v>
       </c>
       <c r="I5" t="s">
         <v>5</v>
@@ -786,8 +840,8 @@
       <c r="K5" t="s">
         <v>5</v>
       </c>
-      <c r="L5">
-        <v>1</v>
+      <c r="L5" t="s">
+        <v>42</v>
       </c>
       <c r="M5" t="s">
         <v>5</v>
@@ -798,8 +852,8 @@
       <c r="O5" t="s">
         <v>5</v>
       </c>
-      <c r="P5">
-        <v>2</v>
+      <c r="P5" t="s">
+        <v>39</v>
       </c>
       <c r="Q5" t="s">
         <v>5</v>
@@ -808,7 +862,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -818,8 +872,8 @@
       <c r="C6" t="s">
         <v>5</v>
       </c>
-      <c r="D6">
-        <v>3</v>
+      <c r="D6" t="s">
+        <v>32</v>
       </c>
       <c r="E6" t="s">
         <v>5</v>
@@ -830,8 +884,8 @@
       <c r="G6" t="s">
         <v>5</v>
       </c>
-      <c r="H6">
-        <v>4</v>
+      <c r="H6" t="s">
+        <v>33</v>
       </c>
       <c r="I6" t="s">
         <v>5</v>
@@ -842,8 +896,8 @@
       <c r="K6" t="s">
         <v>5</v>
       </c>
-      <c r="L6">
-        <v>3</v>
+      <c r="L6" t="s">
+        <v>43</v>
       </c>
       <c r="M6" t="s">
         <v>5</v>
@@ -854,8 +908,8 @@
       <c r="O6" t="s">
         <v>5</v>
       </c>
-      <c r="P6">
-        <v>4</v>
+      <c r="P6" t="s">
+        <v>40</v>
       </c>
       <c r="Q6" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
new version of table
</commit_message>
<xml_diff>
--- a/empty_board.xlsx
+++ b/empty_board.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\03_research_and_development\03_emans_projects\02_my_ideas_and_projects\project_63_sudoku\sudoku_version_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF35B68A-0896-4A57-BB59-063B005EE646}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6C498B4-7113-4B70-B617-CC4676B51D71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{7640EADC-91D7-4D8B-898E-027899374FBD}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{7640EADC-91D7-4D8B-898E-027899374FBD}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="original_idea" sheetId="1" r:id="rId1"/>
+    <sheet name="table" sheetId="2" r:id="rId2"/>
+    <sheet name="mapping" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="60">
   <si>
     <t xml:space="preserve"> ___ ___ ___ ___ </t>
   </si>
@@ -171,6 +172,51 @@
   </si>
   <si>
     <t>TL - P3 - R2 - C3</t>
+  </si>
+  <si>
+    <t>top_left</t>
+  </si>
+  <si>
+    <t>bottom_right</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TR - P1 - R1 - C1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> TL - P3 - R2 - C3 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> BR - P2 - R3 - C2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TR - P3 - R2 - C1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> TL - P1 - R1 - C3 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> BR - P4 - R4 - C2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TR - P4 - R2 - C2 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> TL - P2 - R1 - C4 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> BR - P3 - R4 - C1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TR - P2 - R1 - C2 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> TL - P4 - R2 - C4 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> BR - P1 - R3 - C1</t>
+  </si>
+  <si>
+    <t>top_right</t>
   </si>
 </sst>
 </file>
@@ -573,8 +619,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{056E129C-136F-4364-8967-DD881800EDC5}">
   <dimension ref="A1:R6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P1" sqref="P1:P1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3:H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -922,4 +968,79 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06115EC9-D353-45D6-9B03-48E58C3FE878}">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="172" zoomScaleNormal="172" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="14.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.453125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
created a data frame with all combinations and functions to check 2 rows/cols 3 squares to 4 rows/cols and all frou squares
</commit_message>
<xml_diff>
--- a/empty_board.xlsx
+++ b/empty_board.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\03_research_and_development\03_emans_projects\02_my_ideas_and_projects\project_63_sudoku\sudoku_version_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6C498B4-7113-4B70-B617-CC4676B51D71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{071F40BF-04A2-4C32-9A2D-7E40B947EF90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{7640EADC-91D7-4D8B-898E-027899374FBD}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="3" xr2:uid="{7640EADC-91D7-4D8B-898E-027899374FBD}"/>
   </bookViews>
   <sheets>
     <sheet name="original_idea" sheetId="1" r:id="rId1"/>
     <sheet name="table" sheetId="2" r:id="rId2"/>
     <sheet name="mapping" sheetId="3" r:id="rId3"/>
+    <sheet name="all_possible_combinations" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="64">
   <si>
     <t xml:space="preserve"> ___ ___ ___ ___ </t>
   </si>
@@ -217,6 +218,18 @@
   </si>
   <si>
     <t>top_right</t>
+  </si>
+  <si>
+    <t>v1</t>
+  </si>
+  <si>
+    <t>v2</t>
+  </si>
+  <si>
+    <t>v3</t>
+  </si>
+  <si>
+    <t>v4</t>
   </si>
 </sst>
 </file>
@@ -275,6 +288,22 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6131A606-6676-44DA-A149-734D66071EEB}" name="Table1" displayName="Table1" ref="A1:D25" totalsRowShown="0">
+  <autoFilter ref="A1:D25" xr:uid="{6131A606-6676-44DA-A149-734D66071EEB}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D25">
+    <sortCondition ref="B1:B25"/>
+  </sortState>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{DCBBBFA9-BDDB-47AE-93EB-0A14322B0EE0}" name="v1"/>
+    <tableColumn id="2" xr3:uid="{321150B4-485A-4D0D-B3DC-93015375088E}" name="v2"/>
+    <tableColumn id="3" xr3:uid="{7E38CEF5-2AE4-4320-AF51-6A31856F9C5A}" name="v3"/>
+    <tableColumn id="4" xr3:uid="{BEA4FD29-60DD-4699-B5B1-CD80B3B236E7}" name="v4"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -974,7 +1003,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06115EC9-D353-45D6-9B03-48E58C3FE878}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="172" zoomScaleNormal="172" workbookViewId="0">
+    <sheetView zoomScale="172" zoomScaleNormal="172" workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
@@ -1043,4 +1072,372 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E722FEA8-7A94-4C9C-85F7-056C8BAA0C1B}">
+  <dimension ref="A1:D25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>3</v>
+      </c>
+      <c r="D2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>4</v>
+      </c>
+      <c r="D3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>4</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>3</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>4</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
+      <c r="D7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="C8">
+        <v>3</v>
+      </c>
+      <c r="D8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9">
+        <v>2</v>
+      </c>
+      <c r="C9">
+        <v>4</v>
+      </c>
+      <c r="D9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>3</v>
+      </c>
+      <c r="B10">
+        <v>2</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>3</v>
+      </c>
+      <c r="B11">
+        <v>2</v>
+      </c>
+      <c r="C11">
+        <v>4</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>4</v>
+      </c>
+      <c r="B12">
+        <v>2</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>4</v>
+      </c>
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13">
+        <v>3</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>1</v>
+      </c>
+      <c r="B14">
+        <v>3</v>
+      </c>
+      <c r="C14">
+        <v>4</v>
+      </c>
+      <c r="D14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>1</v>
+      </c>
+      <c r="B15">
+        <v>3</v>
+      </c>
+      <c r="C15">
+        <v>2</v>
+      </c>
+      <c r="D15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <v>2</v>
+      </c>
+      <c r="B16">
+        <v>3</v>
+      </c>
+      <c r="C16">
+        <v>4</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A17">
+        <v>2</v>
+      </c>
+      <c r="B17">
+        <v>3</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A18">
+        <v>4</v>
+      </c>
+      <c r="B18">
+        <v>3</v>
+      </c>
+      <c r="C18">
+        <v>2</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A19">
+        <v>4</v>
+      </c>
+      <c r="B19">
+        <v>3</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A20">
+        <v>1</v>
+      </c>
+      <c r="B20">
+        <v>4</v>
+      </c>
+      <c r="C20">
+        <v>3</v>
+      </c>
+      <c r="D20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A21">
+        <v>1</v>
+      </c>
+      <c r="B21">
+        <v>4</v>
+      </c>
+      <c r="C21">
+        <v>2</v>
+      </c>
+      <c r="D21">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A22">
+        <v>2</v>
+      </c>
+      <c r="B22">
+        <v>4</v>
+      </c>
+      <c r="C22">
+        <v>3</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A23">
+        <v>2</v>
+      </c>
+      <c r="B23">
+        <v>4</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A24">
+        <v>3</v>
+      </c>
+      <c r="B24">
+        <v>4</v>
+      </c>
+      <c r="C24">
+        <v>2</v>
+      </c>
+      <c r="D24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A25">
+        <v>3</v>
+      </c>
+      <c r="B25">
+        <v>4</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="D25">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>